<commit_message>
cleanup of village reach forms
</commit_message>
<xml_diff>
--- a/app/tables/child_coverage/forms/child_coverage/child_coverage.xlsx
+++ b/app/tables/child_coverage/forms/child_coverage/child_coverage.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="6340" windowWidth="20740" windowHeight="11760" tabRatio="439" activeTab="3"/>
+    <workbookView xWindow="1905" yWindow="6345" windowWidth="20730" windowHeight="11760" tabRatio="439"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -895,7 +895,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -997,6 +997,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1020,7 +1027,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1063,6 +1070,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,33 +1381,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="35.5" customWidth="1"/>
-    <col min="10" max="10" width="39.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" customWidth="1"/>
-    <col min="12" max="12" width="41.5" customWidth="1"/>
-    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" customWidth="1"/>
+    <col min="5" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" customWidth="1"/>
+    <col min="10" max="10" width="39.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="41.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="17" width="18.5" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="17" width="18.42578125" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
     <col min="21" max="21" width="27" customWidth="1"/>
-    <col min="22" max="22" width="15.1640625" customWidth="1"/>
-    <col min="23" max="23" width="43.83203125" customWidth="1"/>
+    <col min="22" max="22" width="15.140625" customWidth="1"/>
+    <col min="23" max="23" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17.5" customHeight="1">
+    <row r="1" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
         <v>56</v>
@@ -1466,7 +1476,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="17.5" customHeight="1">
+    <row r="2" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="8" t="s">
@@ -1496,7 +1506,7 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="17.5" customHeight="1">
+    <row r="3" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="D3" s="8"/>
@@ -1525,7 +1535,7 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
     </row>
-    <row r="4" spans="1:23" ht="17.5" customHeight="1">
+    <row r="4" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1556,7 +1566,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="5" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1589,7 +1599,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="6" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1620,7 +1630,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="7" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1653,7 +1663,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="17.5" customHeight="1">
+    <row r="8" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1667,7 +1677,7 @@
       <c r="I8" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="26" t="s">
         <v>250</v>
       </c>
       <c r="K8" s="8"/>
@@ -1686,7 +1696,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="17.5" customHeight="1">
+    <row r="9" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1717,7 +1727,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="10" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1750,7 +1760,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="17.5" customHeight="1">
+    <row r="11" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1781,7 +1791,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="12" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1814,7 +1824,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="17.5" customHeight="1">
+    <row r="13" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1847,7 +1857,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="17.5" customHeight="1">
+    <row r="14" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1880,7 +1890,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="15" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1911,7 +1921,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="16" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1944,7 +1954,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="17.5" customHeight="1">
+    <row r="17" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1975,7 +1985,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="18" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2008,7 +2018,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="17.5" customHeight="1">
+    <row r="19" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G19" s="14" t="s">
         <v>71</v>
       </c>
@@ -2021,7 +2031,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="20" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G20" s="18" t="s">
         <v>197</v>
       </c>
@@ -2036,7 +2046,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="17.5" customHeight="1">
+    <row r="21" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G21" s="23" t="s">
         <v>13</v>
       </c>
@@ -2051,7 +2061,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="22" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G22" s="23" t="s">
         <v>13</v>
       </c>
@@ -2066,7 +2076,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="23" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G23" s="14" t="s">
         <v>71</v>
       </c>
@@ -2079,7 +2089,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="24" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="18" t="s">
         <v>197</v>
       </c>
@@ -2094,7 +2104,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="17.5" customHeight="1">
+    <row r="25" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G25" s="14" t="s">
         <v>71</v>
       </c>
@@ -2107,7 +2117,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="26" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G26" s="18" t="s">
         <v>197</v>
       </c>
@@ -2122,7 +2132,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="17.5" customHeight="1">
+    <row r="27" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G27" s="23" t="s">
         <v>13</v>
       </c>
@@ -2137,7 +2147,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="17.5" customHeight="1">
+    <row r="28" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G28" s="15" t="s">
         <v>71</v>
       </c>
@@ -2150,7 +2160,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="29" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G29" s="18" t="s">
         <v>197</v>
       </c>
@@ -2165,7 +2175,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="17.5" customHeight="1">
+    <row r="30" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G30" s="15" t="s">
         <v>71</v>
       </c>
@@ -2178,7 +2188,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="31" spans="1:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G31" s="18" t="s">
         <v>197</v>
       </c>
@@ -2193,7 +2203,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="17.5" customHeight="1">
+    <row r="32" spans="1:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G32" s="23" t="s">
         <v>13</v>
       </c>
@@ -2208,7 +2218,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="3:23" ht="17.5" customHeight="1">
+    <row r="33" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G33" s="23" t="s">
         <v>13</v>
       </c>
@@ -2223,7 +2233,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="3:23" ht="17.5" customHeight="1">
+    <row r="34" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G34" s="15" t="s">
         <v>71</v>
       </c>
@@ -2236,7 +2246,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="35" spans="3:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G35" s="18" t="s">
         <v>197</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="3:23" ht="17.5" customHeight="1">
+    <row r="36" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G36" s="15" t="s">
         <v>71</v>
       </c>
@@ -2264,7 +2274,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="37" spans="3:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G37" s="18" t="s">
         <v>197</v>
       </c>
@@ -2279,7 +2289,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="3:23" ht="17.5" customHeight="1">
+    <row r="38" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G38" s="23" t="s">
         <v>13</v>
       </c>
@@ -2294,7 +2304,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="3:23" ht="17.5" customHeight="1">
+    <row r="39" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G39" s="15" t="s">
         <v>71</v>
       </c>
@@ -2307,7 +2317,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="40" spans="3:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G40" s="18" t="s">
         <v>197</v>
       </c>
@@ -2322,7 +2332,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="3:23" ht="17.5" customHeight="1">
+    <row r="41" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -2339,7 +2349,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="42" spans="3:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -2358,7 +2368,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="3:23" ht="17.5" customHeight="1">
+    <row r="43" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -2377,7 +2387,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="3:23" ht="17.5" customHeight="1">
+    <row r="44" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -2395,7 +2405,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="3:23" ht="17.5" customHeight="1">
+    <row r="45" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="12"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
@@ -2410,7 +2420,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="46" spans="3:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="12"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
@@ -2428,7 +2438,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="3:23" ht="17.5" customHeight="1">
+    <row r="47" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>71</v>
       </c>
@@ -2439,7 +2449,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="48" spans="3:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G48" s="19" t="s">
         <v>197</v>
       </c>
@@ -2453,7 +2463,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="49" spans="7:23" ht="17.5" customHeight="1">
+    <row r="49" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G49" s="23" t="s">
         <v>13</v>
       </c>
@@ -2469,7 +2479,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="7:23" ht="17.5" customHeight="1">
+    <row r="50" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G50" s="15" t="s">
         <v>71</v>
       </c>
@@ -2482,7 +2492,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="51" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G51" s="18" t="s">
         <v>197</v>
       </c>
@@ -2496,7 +2506,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="52" spans="7:23" ht="17.5" customHeight="1">
+    <row r="52" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G52" s="15" t="s">
         <v>71</v>
       </c>
@@ -2509,7 +2519,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="53" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G53" s="18" t="s">
         <v>197</v>
       </c>
@@ -2523,7 +2533,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="54" spans="7:23" ht="17.5" customHeight="1">
+    <row r="54" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G54" s="23" t="s">
         <v>13</v>
       </c>
@@ -2539,7 +2549,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="7:23" ht="17.5" customHeight="1">
+    <row r="55" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G55" s="6" t="s">
         <v>13</v>
       </c>
@@ -2554,7 +2564,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="56" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G56" s="11" t="s">
         <v>71</v>
       </c>
@@ -2565,7 +2575,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="57" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="57" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G57" s="11" t="s">
         <v>71</v>
       </c>
@@ -2576,7 +2586,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="58" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G58" s="19" t="s">
         <v>197</v>
       </c>
@@ -2590,7 +2600,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="59" spans="7:23" ht="17.5" customHeight="1">
+    <row r="59" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G59" s="11" t="s">
         <v>71</v>
       </c>
@@ -2602,7 +2612,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="60" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G60" s="19" t="s">
         <v>197</v>
       </c>
@@ -2616,7 +2626,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="61" spans="7:23" ht="17.5" customHeight="1">
+    <row r="61" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G61" s="14" t="s">
         <v>71</v>
       </c>
@@ -2628,7 +2638,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="62" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G62" s="18" t="s">
         <v>197</v>
       </c>
@@ -2642,7 +2652,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="7:23" ht="17.5" customHeight="1">
+    <row r="63" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G63" s="23" t="s">
         <v>13</v>
       </c>
@@ -2658,7 +2668,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="7:23" ht="17.5" customHeight="1">
+    <row r="64" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G64" s="15" t="s">
         <v>71</v>
       </c>
@@ -2671,7 +2681,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="65" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G65" s="18" t="s">
         <v>197</v>
       </c>
@@ -2685,7 +2695,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="66" spans="7:23" ht="17.5" customHeight="1">
+    <row r="66" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G66" s="15" t="s">
         <v>71</v>
       </c>
@@ -2698,7 +2708,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="67" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="67" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G67" s="18" t="s">
         <v>197</v>
       </c>
@@ -2712,7 +2722,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="68" spans="7:23" ht="17.5" customHeight="1">
+    <row r="68" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G68" s="6" t="s">
         <v>13</v>
       </c>
@@ -2728,7 +2738,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="69" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="69" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G69" s="6" t="s">
         <v>13</v>
       </c>
@@ -2742,7 +2752,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="70" spans="7:23" ht="17.5" customHeight="1">
+    <row r="70" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G70" s="15" t="s">
         <v>71</v>
       </c>
@@ -2754,7 +2764,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="71" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="71" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G71" s="18" t="s">
         <v>197</v>
       </c>
@@ -2768,7 +2778,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="72" spans="7:23" ht="17.5" customHeight="1">
+    <row r="72" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G72" s="15" t="s">
         <v>71</v>
       </c>
@@ -2780,7 +2790,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="73" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="73" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G73" s="18" t="s">
         <v>197</v>
       </c>
@@ -2794,7 +2804,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="74" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="74" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G74" s="23" t="s">
         <v>13</v>
       </c>
@@ -2809,7 +2819,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="75" spans="7:23" ht="17.5" customHeight="1">
+    <row r="75" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G75" s="15" t="s">
         <v>71</v>
       </c>
@@ -2822,7 +2832,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="76" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G76" s="18" t="s">
         <v>197</v>
       </c>
@@ -2836,7 +2846,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="77" spans="7:23" ht="17.5" customHeight="1">
+    <row r="77" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G77" s="15" t="s">
         <v>71</v>
       </c>
@@ -2849,7 +2859,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="78" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G78" s="18" t="s">
         <v>197</v>
       </c>
@@ -2863,7 +2873,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="79" spans="7:23" ht="17.5" customHeight="1">
+    <row r="79" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G79" s="6" t="s">
         <v>13</v>
       </c>
@@ -2879,7 +2889,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="7:23" ht="17.5" customHeight="1">
+    <row r="80" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G80" s="6" t="s">
         <v>13</v>
       </c>
@@ -2893,7 +2903,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="7:23" ht="17.5" customHeight="1">
+    <row r="81" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
         <v>71</v>
       </c>
@@ -2904,7 +2914,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="82" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="82" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G82" s="19" t="s">
         <v>197</v>
       </c>
@@ -2918,7 +2928,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="83" spans="7:23" ht="17.5" customHeight="1">
+    <row r="83" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
         <v>71</v>
       </c>
@@ -2929,7 +2939,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="84" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G84" s="19" t="s">
         <v>197</v>
       </c>
@@ -2943,7 +2953,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="85" spans="7:23" ht="17.5" customHeight="1">
+    <row r="85" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G85" s="6" t="s">
         <v>13</v>
       </c>
@@ -2958,7 +2968,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="86" spans="7:23" ht="17.5" customHeight="1">
+    <row r="86" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
         <v>71</v>
       </c>
@@ -2970,7 +2980,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="87" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G87" s="19" t="s">
         <v>197</v>
       </c>
@@ -2984,7 +2994,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="88" spans="7:23" ht="17.5" customHeight="1">
+    <row r="88" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
         <v>71</v>
       </c>
@@ -2996,7 +3006,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="89" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="89" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G89" s="19" t="s">
         <v>197</v>
       </c>
@@ -3010,7 +3020,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="90" spans="7:23" ht="17.5" customHeight="1">
+    <row r="90" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G90" s="6" t="s">
         <v>13</v>
       </c>
@@ -3025,7 +3035,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="7:23" ht="17.5" customHeight="1">
+    <row r="91" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G91" s="6" t="s">
         <v>13</v>
       </c>
@@ -3039,7 +3049,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="92" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G92" s="11" t="s">
         <v>71</v>
       </c>
@@ -3050,7 +3060,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="93" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="93" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G93" s="11" t="s">
         <v>71</v>
       </c>
@@ -3061,7 +3071,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="94" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="94" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G94" s="6" t="s">
         <v>197</v>
       </c>
@@ -3075,7 +3085,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="95" spans="7:23" ht="17.5" customHeight="1">
+    <row r="95" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
         <v>71</v>
       </c>
@@ -3086,7 +3096,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="96" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="96" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G96" s="6" t="s">
         <v>197</v>
       </c>
@@ -3100,7 +3110,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="97" spans="7:23" ht="17.5" customHeight="1">
+    <row r="97" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
         <v>71</v>
       </c>
@@ -3111,7 +3121,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="98" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="98" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G98" s="6" t="s">
         <v>197</v>
       </c>
@@ -3125,7 +3135,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="7:23" ht="17.5" customHeight="1">
+    <row r="99" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G99" s="6" t="s">
         <v>13</v>
       </c>
@@ -3140,7 +3150,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="100" spans="7:23" ht="17.5" customHeight="1">
+    <row r="100" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
         <v>71</v>
       </c>
@@ -3152,7 +3162,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="101" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="101" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G101" s="6" t="s">
         <v>197</v>
       </c>
@@ -3166,7 +3176,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="102" spans="7:23" ht="17.5" customHeight="1">
+    <row r="102" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
         <v>71</v>
       </c>
@@ -3178,7 +3188,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="103" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="103" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G103" s="6" t="s">
         <v>197</v>
       </c>
@@ -3192,7 +3202,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="104" spans="7:23" ht="17.5" customHeight="1">
+    <row r="104" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G104" s="6" t="s">
         <v>13</v>
       </c>
@@ -3207,7 +3217,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="105" spans="7:23" ht="17.5" customHeight="1">
+    <row r="105" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G105" s="6" t="s">
         <v>13</v>
       </c>
@@ -3221,7 +3231,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="106" spans="7:23" ht="17.5" customHeight="1">
+    <row r="106" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G106" t="s">
         <v>71</v>
       </c>
@@ -3232,7 +3242,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="107" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G107" s="6" t="s">
         <v>197</v>
       </c>
@@ -3246,7 +3256,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="108" spans="7:23" ht="17.5" customHeight="1">
+    <row r="108" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G108" t="s">
         <v>71</v>
       </c>
@@ -3257,7 +3267,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="109" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="109" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G109" s="6" t="s">
         <v>197</v>
       </c>
@@ -3271,7 +3281,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="110" spans="7:23" ht="17.5" customHeight="1">
+    <row r="110" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G110" s="6" t="s">
         <v>13</v>
       </c>
@@ -3286,7 +3296,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="7:23" ht="17.5" customHeight="1">
+    <row r="111" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G111" t="s">
         <v>71</v>
       </c>
@@ -3298,7 +3308,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="112" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="112" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G112" s="6" t="s">
         <v>197</v>
       </c>
@@ -3312,7 +3322,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="113" spans="7:23" ht="17.5" customHeight="1">
+    <row r="113" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G113" t="s">
         <v>71</v>
       </c>
@@ -3324,7 +3334,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="114" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="114" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G114" s="6" t="s">
         <v>197</v>
       </c>
@@ -3338,7 +3348,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="115" spans="7:23" ht="17.5" customHeight="1">
+    <row r="115" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G115" s="6" t="s">
         <v>13</v>
       </c>
@@ -3353,7 +3363,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="116" spans="7:23" ht="17.5" customHeight="1">
+    <row r="116" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G116" s="6" t="s">
         <v>13</v>
       </c>
@@ -3367,7 +3377,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="7:23" ht="17.5" customHeight="1">
+    <row r="117" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G117" t="s">
         <v>71</v>
       </c>
@@ -3378,7 +3388,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="118" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="118" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G118" s="6" t="s">
         <v>197</v>
       </c>
@@ -3392,7 +3402,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="7:23" ht="17.5" customHeight="1">
+    <row r="119" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G119" t="s">
         <v>71</v>
       </c>
@@ -3403,7 +3413,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="120" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G120" s="6" t="s">
         <v>197</v>
       </c>
@@ -3417,7 +3427,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="121" spans="7:23" ht="17.5" customHeight="1">
+    <row r="121" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G121" s="6" t="s">
         <v>13</v>
       </c>
@@ -3432,7 +3442,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="122" spans="7:23" ht="17.5" customHeight="1">
+    <row r="122" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G122" t="s">
         <v>71</v>
       </c>
@@ -3444,7 +3454,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="123" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="123" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G123" s="6" t="s">
         <v>197</v>
       </c>
@@ -3458,7 +3468,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="124" spans="7:23" ht="17.5" customHeight="1">
+    <row r="124" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G124" t="s">
         <v>71</v>
       </c>
@@ -3470,7 +3480,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="125" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="125" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G125" s="6" t="s">
         <v>197</v>
       </c>
@@ -3484,7 +3494,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="126" spans="7:23" ht="17.5" customHeight="1">
+    <row r="126" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G126" s="6" t="s">
         <v>13</v>
       </c>
@@ -3499,7 +3509,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="127" spans="7:23" ht="17.5" customHeight="1">
+    <row r="127" spans="7:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G127" s="6" t="s">
         <v>13</v>
       </c>
@@ -3513,7 +3523,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="7:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="128" spans="7:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G128" s="11" t="s">
         <v>71</v>
       </c>
@@ -3527,7 +3537,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="129" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="129" spans="3:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G129" s="19" t="s">
         <v>197</v>
       </c>
@@ -3541,7 +3551,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="130" spans="3:23" ht="17.5" customHeight="1">
+    <row r="130" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G130" t="s">
         <v>71</v>
       </c>
@@ -3552,7 +3562,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="131" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="131" spans="3:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G131" s="19" t="s">
         <v>197</v>
       </c>
@@ -3566,7 +3576,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="132" spans="3:23" ht="17.5" customHeight="1">
+    <row r="132" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G132" t="s">
         <v>71</v>
       </c>
@@ -3577,7 +3587,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="133" spans="3:23" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="133" spans="3:23" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G133" s="19" t="s">
         <v>197</v>
       </c>
@@ -3591,7 +3601,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="134" spans="3:23" ht="17.5" customHeight="1">
+    <row r="134" spans="3:23" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G134" s="6" t="s">
         <v>13</v>
       </c>
@@ -3606,7 +3616,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="135" spans="3:23" ht="12.75" customHeight="1">
+    <row r="135" spans="3:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G135" t="s">
         <v>71</v>
       </c>
@@ -3618,7 +3628,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="136" spans="3:23" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="136" spans="3:23" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G136" s="19" t="s">
         <v>197</v>
       </c>
@@ -3632,7 +3642,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="137" spans="3:23" ht="12.75" customHeight="1">
+    <row r="137" spans="3:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G137" t="s">
         <v>71</v>
       </c>
@@ -3644,7 +3654,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="138" spans="3:23" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="138" spans="3:23" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G138" s="19" t="s">
         <v>197</v>
       </c>
@@ -3658,7 +3668,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="139" spans="3:23" ht="12.75" customHeight="1">
+    <row r="139" spans="3:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G139" s="6" t="s">
         <v>13</v>
       </c>
@@ -3673,7 +3683,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="140" spans="3:23" ht="12.75" customHeight="1">
+    <row r="140" spans="3:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G140" s="6" t="s">
         <v>13</v>
       </c>
@@ -3687,7 +3697,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="141" spans="3:23" ht="12.75" customHeight="1">
+    <row r="141" spans="3:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G141" t="s">
         <v>71</v>
       </c>
@@ -3698,7 +3708,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="142" spans="3:23" ht="12.75" customHeight="1">
+    <row r="142" spans="3:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G142" s="19" t="s">
         <v>197</v>
       </c>
@@ -3712,14 +3722,14 @@
         <v>212</v>
       </c>
     </row>
-    <row r="143" spans="3:23" ht="12.75" customHeight="1">
+    <row r="143" spans="3:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C143" s="11" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3733,16 +3743,16 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="127.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="127.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" customHeight="1">
+    <row r="1" spans="1:2" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -3750,7 +3760,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="11" customFormat="1" ht="17.5" customHeight="1">
+    <row r="2" spans="1:2" s="11" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>74</v>
       </c>
@@ -3758,7 +3768,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.75" customHeight="1">
+    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -3766,7 +3776,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.75" customHeight="1">
+    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>77</v>
       </c>
@@ -3774,7 +3784,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="11" customFormat="1" ht="12.75" customHeight="1">
+    <row r="5" spans="1:2" s="11" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>82</v>
       </c>
@@ -3782,7 +3792,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12.75" customHeight="1">
+    <row r="6" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>83</v>
       </c>
@@ -3790,7 +3800,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="12.75" customHeight="1">
+    <row r="7" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -3798,7 +3808,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="12.75" customHeight="1">
+    <row r="8" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -3806,7 +3816,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="12.75" customHeight="1">
+    <row r="9" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>90</v>
       </c>
@@ -3814,7 +3824,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="12.75" customHeight="1">
+    <row r="10" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>93</v>
       </c>
@@ -3822,7 +3832,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="12.75" customHeight="1">
+    <row r="11" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>96</v>
       </c>
@@ -3830,7 +3840,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="12.75" customHeight="1">
+    <row r="12" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>97</v>
       </c>
@@ -3838,7 +3848,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="12.75" customHeight="1">
+    <row r="13" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>100</v>
       </c>
@@ -3846,7 +3856,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="12.75" customHeight="1">
+    <row r="14" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>103</v>
       </c>
@@ -3854,7 +3864,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="12.75" customHeight="1">
+    <row r="15" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>104</v>
       </c>
@@ -3862,7 +3872,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="12.75" customHeight="1">
+    <row r="16" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -3870,7 +3880,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="12.75" customHeight="1">
+    <row r="17" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -3878,7 +3888,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="12.75" customHeight="1">
+    <row r="18" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -3886,7 +3896,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="12.75" customHeight="1">
+    <row r="19" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>116</v>
       </c>
@@ -3894,7 +3904,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="12.75" customHeight="1">
+    <row r="20" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>113</v>
       </c>
@@ -3902,7 +3912,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="12.75" customHeight="1">
+    <row r="21" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>112</v>
       </c>
@@ -3910,7 +3920,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="12.75" customHeight="1">
+    <row r="22" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>121</v>
       </c>
@@ -3918,7 +3928,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="12.75" customHeight="1">
+    <row r="23" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>124</v>
       </c>
@@ -3926,7 +3936,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="12.75" customHeight="1">
+    <row r="24" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>125</v>
       </c>
@@ -3934,7 +3944,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="12.75" customHeight="1">
+    <row r="25" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>144</v>
       </c>
@@ -3942,7 +3952,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="12.75" customHeight="1">
+    <row r="26" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>141</v>
       </c>
@@ -3950,7 +3960,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="12.75" customHeight="1">
+    <row r="27" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>140</v>
       </c>
@@ -3958,7 +3968,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="12.75" customHeight="1">
+    <row r="28" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>137</v>
       </c>
@@ -3966,7 +3976,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="12.75" customHeight="1">
+    <row r="29" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>134</v>
       </c>
@@ -3974,7 +3984,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="12.75" customHeight="1">
+    <row r="30" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>133</v>
       </c>
@@ -3982,7 +3992,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="12.75" customHeight="1">
+    <row r="31" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>130</v>
       </c>
@@ -3990,7 +4000,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="12.75" customHeight="1">
+    <row r="32" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>127</v>
       </c>
@@ -3998,7 +4008,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="12.75" customHeight="1">
+    <row r="33" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>126</v>
       </c>
@@ -4006,7 +4016,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="12.75" customHeight="1">
+    <row r="34" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>151</v>
       </c>
@@ -4014,7 +4024,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="12.75" customHeight="1">
+    <row r="35" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>152</v>
       </c>
@@ -4022,7 +4032,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="12.75" customHeight="1">
+    <row r="36" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>153</v>
       </c>
@@ -4048,14 +4058,14 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" customHeight="1">
+    <row r="1" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -4066,7 +4076,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.5" customHeight="1">
+    <row r="2" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -4077,7 +4087,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" customHeight="1">
+    <row r="3" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -4088,7 +4098,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" customHeight="1">
+    <row r="4" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -4099,7 +4109,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" customHeight="1">
+    <row r="5" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -4110,7 +4120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.5" customHeight="1">
+    <row r="6" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -4121,7 +4131,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.5" customHeight="1">
+    <row r="7" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -4132,7 +4142,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.5" customHeight="1">
+    <row r="8" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -4143,7 +4153,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.5" customHeight="1">
+    <row r="9" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -4154,7 +4164,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.5" customHeight="1">
+    <row r="10" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -4165,8 +4175,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="12" spans="1:3" ht="17.5" customHeight="1">
+    <row r="11" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4177,7 +4187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.5" customHeight="1">
+    <row r="13" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -4188,7 +4198,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.5" customHeight="1">
+    <row r="14" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -4199,7 +4209,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.5" customHeight="1">
+    <row r="15" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -4210,7 +4220,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.5" customHeight="1">
+    <row r="16" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4221,7 +4231,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5" customHeight="1">
+    <row r="17" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -4232,7 +4242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.5" customHeight="1">
+    <row r="18" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -4243,7 +4253,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.5" customHeight="1">
+    <row r="19" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -4254,7 +4264,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.5" customHeight="1">
+    <row r="20" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -4265,7 +4275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.5" customHeight="1">
+    <row r="21" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -4276,8 +4286,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="23" spans="1:3" ht="17.5" customHeight="1">
+    <row r="22" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -4288,7 +4298,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.5" customHeight="1">
+    <row r="24" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -4299,8 +4309,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.5" customHeight="1"/>
-    <row r="26" spans="1:3" ht="17.5" customHeight="1">
+    <row r="25" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>66</v>
       </c>
@@ -4311,7 +4321,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="12.75" customHeight="1">
+    <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>66</v>
       </c>
@@ -4322,7 +4332,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="12.75" customHeight="1">
+    <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>66</v>
       </c>
@@ -4333,7 +4343,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="12.75" customHeight="1">
+    <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>196</v>
       </c>
@@ -4358,18 +4368,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1">
+    <row r="1" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -4380,7 +4390,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.5" customHeight="1">
+    <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -4388,7 +4398,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.5" customHeight="1">
+    <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
@@ -4396,7 +4406,7 @@
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" customHeight="1">
+    <row r="4" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -4404,7 +4414,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.5" customHeight="1">
+    <row r="5" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>288</v>
       </c>
@@ -4412,8 +4422,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
-    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="6" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>